<commit_message>
Init - added selenium based automation
</commit_message>
<xml_diff>
--- a/src/main/resources/membersList.xlsx
+++ b/src/main/resources/membersList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,21 +28,33 @@
     <t xml:space="preserve">Platform</t>
   </si>
   <si>
-    <t xml:space="preserve">A5P3CT_ZA</t>
+    <t xml:space="preserve">Alexvomits</t>
   </si>
   <si>
     <t xml:space="preserve">epic</t>
   </si>
   <si>
+    <t xml:space="preserve">Anubisgoat1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Army gunners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVN7</t>
+  </si>
+  <si>
     <t xml:space="preserve">BeerMasjien</t>
   </si>
   <si>
-    <t xml:space="preserve">Bybear126</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bobman2947</t>
   </si>
   <si>
+    <t xml:space="preserve">xbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRO_Dragaawn</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chutney_Tjops</t>
   </si>
   <si>
@@ -52,22 +64,25 @@
     <t xml:space="preserve">daCostaRaps</t>
   </si>
   <si>
+    <t xml:space="preserve">psn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eskapa1d</t>
+  </si>
+  <si>
     <t xml:space="preserve">FiNniCKin_2Jz</t>
   </si>
   <si>
-    <t xml:space="preserve">psn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GhostRapter1415</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xbl</t>
+    <t xml:space="preserve">GreenDragon0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannib8l OG</t>
   </si>
   <si>
     <t xml:space="preserve">HerezAJoHnnY</t>
   </si>
   <si>
-    <t xml:space="preserve">JamalVanDuk3</t>
+    <t xml:space="preserve">Jamalvandux</t>
   </si>
   <si>
     <t xml:space="preserve">Japes360</t>
@@ -76,31 +91,61 @@
     <t xml:space="preserve">K1LL1NGF13LD5</t>
   </si>
   <si>
+    <t xml:space="preserve">KillerPranesh</t>
+  </si>
+  <si>
     <t xml:space="preserve">MightyMidget8811</t>
   </si>
   <si>
+    <t xml:space="preserve">MonsterGames200</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mr_Ballistic_</t>
   </si>
   <si>
     <t xml:space="preserve">Nanashi_ZA</t>
   </si>
   <si>
+    <t xml:space="preserve">NaVeDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoNoob1415</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oops123rage</t>
   </si>
   <si>
     <t xml:space="preserve">Reckless_ness11</t>
   </si>
   <si>
-    <t xml:space="preserve">RMAC1294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SaneSeraph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sup_G19</t>
+    <t xml:space="preserve">Rusting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SONIC-_1397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sweetdreamcringe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TakenPersonally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THAPZIN_6</t>
   </si>
   <si>
     <t xml:space="preserve">TheBromeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turtlejuice 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wasabi_ZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZeroTwo0_ </t>
   </si>
 </sst>
 </file>
@@ -202,7 +247,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -266,12 +311,12 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -279,10 +324,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,15 +335,15 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,7 +351,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,7 +359,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,7 +399,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,7 +415,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,7 +423,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,7 +439,127 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>